<commit_message>
Update Leave Card 6/9/2023 10:23 PM
</commit_message>
<xml_diff>
--- a/REGULAR/OJT/NEW DONE/FERMA, ELIZA.xlsx
+++ b/REGULAR/OJT/NEW DONE/FERMA, ELIZA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVONITALLA FAMILY\Desktop\LEAVECARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\REGULAR\OJT\NEW DONE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7D33EE-7561-43BC-A5F9-22D1ACA1139C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -24,25 +25,17 @@
     <definedName name="BALANCE_1">Table1[[#Headers],[BALANCE]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Sheet1!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="133">
   <si>
     <t>PERIOD</t>
   </si>
@@ -411,12 +404,42 @@
   </si>
   <si>
     <t>04/7-15/2018</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>SL(10-0-0)</t>
+  </si>
+  <si>
+    <t>SL(20-0-0)</t>
+  </si>
+  <si>
+    <t>1/31 - 2/9/2023</t>
+  </si>
+  <si>
+    <t>2/10 - 3/1/2023</t>
+  </si>
+  <si>
+    <t>5/27/1996</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -786,6 +809,12 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -821,12 +850,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1276,7 +1299,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1319,7 +1342,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1383,7 +1406,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1443,7 +1466,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1509,7 +1532,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1572,7 +1595,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1670,7 +1693,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1729,7 +1752,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1794,7 +1817,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1837,7 +1860,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1912,7 +1935,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2098,7 +2121,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2164,7 +2187,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2222,7 +2245,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2288,7 +2311,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2344,7 +2367,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2419,7 +2442,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2462,7 +2485,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2528,7 +2551,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2584,7 +2607,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2682,7 +2705,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2745,7 +2768,7 @@
         <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2794,7 +2817,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2811,25 +2834,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K318" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A8:K381" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="20"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="19"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="18"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="17"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="16">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="15"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="14">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="13"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="12">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="12">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="11"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2841,13 +2864,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D2:G3" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="D2:G3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="D2:G3" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="D2:G3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="DAYS"/>
-    <tableColumn id="2" name="HOURS"/>
-    <tableColumn id="3" name="MINUTES"/>
-    <tableColumn id="4" name="EQUIVALENT HOURS" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="DAYS"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="HOURS"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="MINUTES"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="EQUIVALENT HOURS" dataDxfId="5">
       <calculatedColumnFormula>SUMIFS(F7:F14,E7:E14,E3)+SUMIFS(D7:D66,C7:C66,F3)+D3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2856,14 +2879,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="J2:L3" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="J2:L3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="J2:L3" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="J2:L3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="DATE STARTED" dataDxfId="2"/>
-    <tableColumn id="2" name="LEAVE EARN" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="DATE STARTED" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="LEAVE EARN" dataDxfId="1">
       <calculatedColumnFormula>J4-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="LEAVE EARNED" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="LEAVE EARNED" dataDxfId="0">
       <calculatedColumnFormula>IF($J$4=1,1.25,IF(ISBLANK($J$3),"---",1.25-VLOOKUP($K$3,$I$8:$K$37,2)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3167,7 +3190,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -3185,16 +3208,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K318"/>
+  <dimension ref="A2:K381"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4152" topLeftCell="A141" activePane="bottomLeft"/>
+      <pane ySplit="4152" topLeftCell="A4" activePane="bottomLeft"/>
       <selection activeCell="B2" sqref="B2:C2"/>
-      <selection pane="bottomLeft" activeCell="A273" sqref="A273"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3216,58 +3239,60 @@
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="49"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="51"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="54"/>
+      <c r="F3" s="59" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="56"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="55"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -3293,18 +3318,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48" t="s">
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -3351,7 +3376,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>178.31100000000001</v>
+        <v>229.56100000000001</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3361,13 +3386,13 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>303.517</v>
+        <v>349.767</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="48" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="20"/>
@@ -3429,7 +3454,7 @@
       <c r="K12" s="20"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="48" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="20"/>
@@ -3517,7 +3542,7 @@
       <c r="K16" s="15"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="48" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="20"/>
@@ -3779,7 +3804,7 @@
       <c r="K29" s="20"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="60" t="s">
+      <c r="A30" s="48" t="s">
         <v>54</v>
       </c>
       <c r="B30" s="20"/>
@@ -4045,7 +4070,7 @@
       <c r="K42" s="20"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="60" t="s">
+      <c r="A43" s="48" t="s">
         <v>55</v>
       </c>
       <c r="B43" s="20"/>
@@ -4325,7 +4350,7 @@
       <c r="K55" s="20"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A56" s="60" t="s">
+      <c r="A56" s="48" t="s">
         <v>56</v>
       </c>
       <c r="B56" s="20"/>
@@ -4629,7 +4654,7 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A69" s="60" t="s">
+      <c r="A69" s="48" t="s">
         <v>57</v>
       </c>
       <c r="B69" s="20"/>
@@ -5017,7 +5042,7 @@
       <c r="K85" s="20"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A86" s="60" t="s">
+      <c r="A86" s="48" t="s">
         <v>104</v>
       </c>
       <c r="B86" s="20"/>
@@ -5285,7 +5310,7 @@
       <c r="K98" s="20"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A99" s="60" t="s">
+      <c r="A99" s="48" t="s">
         <v>103</v>
       </c>
       <c r="B99" s="20"/>
@@ -5557,7 +5582,7 @@
       <c r="K111" s="20"/>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A112" s="60" t="s">
+      <c r="A112" s="48" t="s">
         <v>102</v>
       </c>
       <c r="B112" s="20"/>
@@ -5825,7 +5850,7 @@
       <c r="K124" s="20"/>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A125" s="60" t="s">
+      <c r="A125" s="48" t="s">
         <v>101</v>
       </c>
       <c r="B125" s="20"/>
@@ -6119,7 +6144,7 @@
       <c r="K138" s="20"/>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A139" s="60" t="s">
+      <c r="A139" s="48" t="s">
         <v>100</v>
       </c>
       <c r="B139" s="20"/>
@@ -6419,7 +6444,7 @@
       <c r="K152" s="20"/>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A153" s="60" t="s">
+      <c r="A153" s="48" t="s">
         <v>99</v>
       </c>
       <c r="B153" s="20"/>
@@ -6685,7 +6710,7 @@
       <c r="K165" s="20"/>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A166" s="60" t="s">
+      <c r="A166" s="48" t="s">
         <v>98</v>
       </c>
       <c r="B166" s="20"/>
@@ -6971,7 +6996,7 @@
       <c r="K179" s="20"/>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A180" s="60" t="s">
+      <c r="A180" s="48" t="s">
         <v>97</v>
       </c>
       <c r="B180" s="20"/>
@@ -7233,7 +7258,7 @@
       <c r="K192" s="20"/>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A193" s="60" t="s">
+      <c r="A193" s="48" t="s">
         <v>96</v>
       </c>
       <c r="B193" s="20"/>
@@ -7499,7 +7524,7 @@
       <c r="K205" s="20"/>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A206" s="60" t="s">
+      <c r="A206" s="48" t="s">
         <v>95</v>
       </c>
       <c r="B206" s="20"/>
@@ -7765,7 +7790,7 @@
       <c r="K218" s="20"/>
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A219" s="60" t="s">
+      <c r="A219" s="48" t="s">
         <v>94</v>
       </c>
       <c r="B219" s="20"/>
@@ -8031,7 +8056,7 @@
       <c r="K231" s="20"/>
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A232" s="60" t="s">
+      <c r="A232" s="48" t="s">
         <v>93</v>
       </c>
       <c r="B232" s="20"/>
@@ -8297,7 +8322,7 @@
       <c r="K244" s="20"/>
     </row>
     <row r="245" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A245" s="60" t="s">
+      <c r="A245" s="48" t="s">
         <v>92</v>
       </c>
       <c r="B245" s="20"/>
@@ -8563,7 +8588,7 @@
       <c r="K257" s="20"/>
     </row>
     <row r="258" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A258" s="60" t="s">
+      <c r="A258" s="48" t="s">
         <v>91</v>
       </c>
       <c r="B258" s="20"/>
@@ -8829,7 +8854,7 @@
       <c r="K270" s="20"/>
     </row>
     <row r="271" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A271" s="60" t="s">
+      <c r="A271" s="48" t="s">
         <v>90</v>
       </c>
       <c r="B271" s="20"/>
@@ -9099,7 +9124,7 @@
       <c r="K283" s="20"/>
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A284" s="60" t="s">
+      <c r="A284" s="48" t="s">
         <v>120</v>
       </c>
       <c r="B284" s="20"/>
@@ -9202,20 +9227,24 @@
       </c>
       <c r="I288" s="9"/>
       <c r="J288" s="11"/>
-      <c r="K288" s="61" t="s">
+      <c r="K288" s="49" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="289" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A289" s="40"/>
+      <c r="A289" s="40">
+        <v>43221</v>
+      </c>
       <c r="B289" s="20"/>
-      <c r="C289" s="13"/>
+      <c r="C289" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D289" s="39"/>
       <c r="E289" s="9"/>
       <c r="F289" s="20"/>
-      <c r="G289" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G289" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H289" s="39"/>
       <c r="I289" s="9"/>
@@ -9223,15 +9252,19 @@
       <c r="K289" s="20"/>
     </row>
     <row r="290" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A290" s="40"/>
+      <c r="A290" s="40">
+        <v>43252</v>
+      </c>
       <c r="B290" s="20"/>
-      <c r="C290" s="13"/>
+      <c r="C290" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D290" s="39"/>
       <c r="E290" s="9"/>
       <c r="F290" s="20"/>
-      <c r="G290" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G290" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H290" s="39"/>
       <c r="I290" s="9"/>
@@ -9239,15 +9272,19 @@
       <c r="K290" s="20"/>
     </row>
     <row r="291" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A291" s="40"/>
+      <c r="A291" s="40">
+        <v>43282</v>
+      </c>
       <c r="B291" s="20"/>
-      <c r="C291" s="13"/>
+      <c r="C291" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D291" s="39"/>
       <c r="E291" s="9"/>
       <c r="F291" s="20"/>
-      <c r="G291" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G291" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H291" s="39"/>
       <c r="I291" s="9"/>
@@ -9255,15 +9292,19 @@
       <c r="K291" s="20"/>
     </row>
     <row r="292" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A292" s="40"/>
+      <c r="A292" s="40">
+        <v>43313</v>
+      </c>
       <c r="B292" s="20"/>
-      <c r="C292" s="13"/>
+      <c r="C292" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D292" s="39"/>
       <c r="E292" s="9"/>
       <c r="F292" s="20"/>
-      <c r="G292" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G292" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H292" s="39"/>
       <c r="I292" s="9"/>
@@ -9271,15 +9312,19 @@
       <c r="K292" s="20"/>
     </row>
     <row r="293" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A293" s="40"/>
+      <c r="A293" s="40">
+        <v>43344</v>
+      </c>
       <c r="B293" s="20"/>
-      <c r="C293" s="13"/>
+      <c r="C293" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D293" s="39"/>
       <c r="E293" s="9"/>
       <c r="F293" s="20"/>
-      <c r="G293" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G293" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H293" s="39"/>
       <c r="I293" s="9"/>
@@ -9287,15 +9332,19 @@
       <c r="K293" s="20"/>
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A294" s="40"/>
+      <c r="A294" s="40">
+        <v>43374</v>
+      </c>
       <c r="B294" s="20"/>
-      <c r="C294" s="13"/>
+      <c r="C294" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D294" s="39"/>
       <c r="E294" s="9"/>
       <c r="F294" s="20"/>
-      <c r="G294" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G294" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H294" s="39"/>
       <c r="I294" s="9"/>
@@ -9303,15 +9352,19 @@
       <c r="K294" s="20"/>
     </row>
     <row r="295" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A295" s="40"/>
+      <c r="A295" s="40">
+        <v>43405</v>
+      </c>
       <c r="B295" s="20"/>
-      <c r="C295" s="13"/>
+      <c r="C295" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D295" s="39"/>
       <c r="E295" s="9"/>
       <c r="F295" s="20"/>
-      <c r="G295" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G295" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H295" s="39"/>
       <c r="I295" s="9"/>
@@ -9319,15 +9372,23 @@
       <c r="K295" s="20"/>
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A296" s="40"/>
-      <c r="B296" s="20"/>
-      <c r="C296" s="13"/>
-      <c r="D296" s="39"/>
+      <c r="A296" s="40">
+        <v>43435</v>
+      </c>
+      <c r="B296" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C296" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D296" s="39">
+        <v>5</v>
+      </c>
       <c r="E296" s="9"/>
       <c r="F296" s="20"/>
-      <c r="G296" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G296" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H296" s="39"/>
       <c r="I296" s="9"/>
@@ -9335,7 +9396,9 @@
       <c r="K296" s="20"/>
     </row>
     <row r="297" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A297" s="40"/>
+      <c r="A297" s="48" t="s">
+        <v>124</v>
+      </c>
       <c r="B297" s="20"/>
       <c r="C297" s="13"/>
       <c r="D297" s="39"/>
@@ -9351,15 +9414,19 @@
       <c r="K297" s="20"/>
     </row>
     <row r="298" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A298" s="40"/>
+      <c r="A298" s="40">
+        <v>43466</v>
+      </c>
       <c r="B298" s="20"/>
-      <c r="C298" s="13"/>
+      <c r="C298" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D298" s="39"/>
       <c r="E298" s="9"/>
       <c r="F298" s="20"/>
-      <c r="G298" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G298" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H298" s="39"/>
       <c r="I298" s="9"/>
@@ -9367,15 +9434,19 @@
       <c r="K298" s="20"/>
     </row>
     <row r="299" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A299" s="40"/>
+      <c r="A299" s="40">
+        <v>43497</v>
+      </c>
       <c r="B299" s="20"/>
-      <c r="C299" s="13"/>
+      <c r="C299" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D299" s="39"/>
       <c r="E299" s="9"/>
       <c r="F299" s="20"/>
-      <c r="G299" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G299" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H299" s="39"/>
       <c r="I299" s="9"/>
@@ -9383,15 +9454,19 @@
       <c r="K299" s="20"/>
     </row>
     <row r="300" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A300" s="40"/>
+      <c r="A300" s="40">
+        <v>43525</v>
+      </c>
       <c r="B300" s="20"/>
-      <c r="C300" s="13"/>
+      <c r="C300" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D300" s="39"/>
       <c r="E300" s="9"/>
       <c r="F300" s="20"/>
-      <c r="G300" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G300" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H300" s="39"/>
       <c r="I300" s="9"/>
@@ -9399,15 +9474,19 @@
       <c r="K300" s="20"/>
     </row>
     <row r="301" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A301" s="40"/>
+      <c r="A301" s="40">
+        <v>43556</v>
+      </c>
       <c r="B301" s="20"/>
-      <c r="C301" s="13"/>
+      <c r="C301" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D301" s="39"/>
       <c r="E301" s="9"/>
       <c r="F301" s="20"/>
-      <c r="G301" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G301" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H301" s="39"/>
       <c r="I301" s="9"/>
@@ -9415,15 +9494,19 @@
       <c r="K301" s="20"/>
     </row>
     <row r="302" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A302" s="40"/>
+      <c r="A302" s="40">
+        <v>43586</v>
+      </c>
       <c r="B302" s="20"/>
-      <c r="C302" s="13"/>
+      <c r="C302" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D302" s="39"/>
       <c r="E302" s="9"/>
       <c r="F302" s="20"/>
-      <c r="G302" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G302" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H302" s="39"/>
       <c r="I302" s="9"/>
@@ -9431,15 +9514,19 @@
       <c r="K302" s="20"/>
     </row>
     <row r="303" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A303" s="40"/>
+      <c r="A303" s="40">
+        <v>43617</v>
+      </c>
       <c r="B303" s="20"/>
-      <c r="C303" s="13"/>
+      <c r="C303" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D303" s="39"/>
       <c r="E303" s="9"/>
       <c r="F303" s="20"/>
-      <c r="G303" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G303" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H303" s="39"/>
       <c r="I303" s="9"/>
@@ -9447,15 +9534,19 @@
       <c r="K303" s="20"/>
     </row>
     <row r="304" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A304" s="40"/>
+      <c r="A304" s="40">
+        <v>43647</v>
+      </c>
       <c r="B304" s="20"/>
-      <c r="C304" s="13"/>
+      <c r="C304" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D304" s="39"/>
       <c r="E304" s="9"/>
       <c r="F304" s="20"/>
-      <c r="G304" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G304" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H304" s="39"/>
       <c r="I304" s="9"/>
@@ -9463,15 +9554,19 @@
       <c r="K304" s="20"/>
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A305" s="40"/>
+      <c r="A305" s="40">
+        <v>43678</v>
+      </c>
       <c r="B305" s="20"/>
-      <c r="C305" s="13"/>
+      <c r="C305" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D305" s="39"/>
       <c r="E305" s="9"/>
       <c r="F305" s="20"/>
-      <c r="G305" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G305" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H305" s="39"/>
       <c r="I305" s="9"/>
@@ -9479,15 +9574,19 @@
       <c r="K305" s="20"/>
     </row>
     <row r="306" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A306" s="40"/>
+      <c r="A306" s="40">
+        <v>43709</v>
+      </c>
       <c r="B306" s="20"/>
-      <c r="C306" s="13"/>
+      <c r="C306" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D306" s="39"/>
       <c r="E306" s="9"/>
       <c r="F306" s="20"/>
-      <c r="G306" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G306" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H306" s="39"/>
       <c r="I306" s="9"/>
@@ -9495,15 +9594,19 @@
       <c r="K306" s="20"/>
     </row>
     <row r="307" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A307" s="40"/>
+      <c r="A307" s="40">
+        <v>43739</v>
+      </c>
       <c r="B307" s="20"/>
-      <c r="C307" s="13"/>
+      <c r="C307" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D307" s="39"/>
       <c r="E307" s="9"/>
       <c r="F307" s="20"/>
-      <c r="G307" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G307" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H307" s="39"/>
       <c r="I307" s="9"/>
@@ -9511,15 +9614,19 @@
       <c r="K307" s="20"/>
     </row>
     <row r="308" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A308" s="40"/>
+      <c r="A308" s="40">
+        <v>43770</v>
+      </c>
       <c r="B308" s="20"/>
-      <c r="C308" s="13"/>
+      <c r="C308" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D308" s="39"/>
       <c r="E308" s="9"/>
       <c r="F308" s="20"/>
-      <c r="G308" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G308" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H308" s="39"/>
       <c r="I308" s="9"/>
@@ -9527,15 +9634,23 @@
       <c r="K308" s="20"/>
     </row>
     <row r="309" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A309" s="40"/>
-      <c r="B309" s="20"/>
-      <c r="C309" s="13"/>
-      <c r="D309" s="39"/>
+      <c r="A309" s="40">
+        <v>43800</v>
+      </c>
+      <c r="B309" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C309" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D309" s="39">
+        <v>5</v>
+      </c>
       <c r="E309" s="9"/>
       <c r="F309" s="20"/>
-      <c r="G309" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G309" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H309" s="39"/>
       <c r="I309" s="9"/>
@@ -9543,7 +9658,9 @@
       <c r="K309" s="20"/>
     </row>
     <row r="310" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A310" s="40"/>
+      <c r="A310" s="48" t="s">
+        <v>125</v>
+      </c>
       <c r="B310" s="20"/>
       <c r="C310" s="13"/>
       <c r="D310" s="39"/>
@@ -9559,15 +9676,19 @@
       <c r="K310" s="20"/>
     </row>
     <row r="311" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A311" s="40"/>
+      <c r="A311" s="40">
+        <v>43831</v>
+      </c>
       <c r="B311" s="20"/>
-      <c r="C311" s="13"/>
+      <c r="C311" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D311" s="39"/>
       <c r="E311" s="9"/>
       <c r="F311" s="20"/>
-      <c r="G311" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G311" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H311" s="39"/>
       <c r="I311" s="9"/>
@@ -9575,15 +9696,19 @@
       <c r="K311" s="20"/>
     </row>
     <row r="312" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A312" s="40"/>
+      <c r="A312" s="40">
+        <v>43862</v>
+      </c>
       <c r="B312" s="20"/>
-      <c r="C312" s="13"/>
+      <c r="C312" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D312" s="39"/>
       <c r="E312" s="9"/>
       <c r="F312" s="20"/>
-      <c r="G312" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G312" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H312" s="39"/>
       <c r="I312" s="9"/>
@@ -9591,15 +9716,19 @@
       <c r="K312" s="20"/>
     </row>
     <row r="313" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A313" s="40"/>
+      <c r="A313" s="40">
+        <v>43891</v>
+      </c>
       <c r="B313" s="20"/>
-      <c r="C313" s="13"/>
+      <c r="C313" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D313" s="39"/>
       <c r="E313" s="9"/>
       <c r="F313" s="20"/>
-      <c r="G313" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G313" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H313" s="39"/>
       <c r="I313" s="9"/>
@@ -9607,15 +9736,19 @@
       <c r="K313" s="20"/>
     </row>
     <row r="314" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A314" s="40"/>
+      <c r="A314" s="40">
+        <v>43922</v>
+      </c>
       <c r="B314" s="20"/>
-      <c r="C314" s="13"/>
+      <c r="C314" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D314" s="39"/>
       <c r="E314" s="9"/>
       <c r="F314" s="20"/>
-      <c r="G314" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G314" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H314" s="39"/>
       <c r="I314" s="9"/>
@@ -9623,15 +9756,19 @@
       <c r="K314" s="20"/>
     </row>
     <row r="315" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A315" s="40"/>
+      <c r="A315" s="40">
+        <v>43952</v>
+      </c>
       <c r="B315" s="20"/>
-      <c r="C315" s="13"/>
+      <c r="C315" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D315" s="39"/>
       <c r="E315" s="9"/>
       <c r="F315" s="20"/>
-      <c r="G315" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G315" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H315" s="39"/>
       <c r="I315" s="9"/>
@@ -9639,15 +9776,19 @@
       <c r="K315" s="20"/>
     </row>
     <row r="316" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A316" s="40"/>
+      <c r="A316" s="40">
+        <v>43983</v>
+      </c>
       <c r="B316" s="20"/>
-      <c r="C316" s="13"/>
+      <c r="C316" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D316" s="39"/>
       <c r="E316" s="9"/>
       <c r="F316" s="20"/>
-      <c r="G316" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G316" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H316" s="39"/>
       <c r="I316" s="9"/>
@@ -9655,15 +9796,19 @@
       <c r="K316" s="20"/>
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A317" s="40"/>
+      <c r="A317" s="40">
+        <v>44013</v>
+      </c>
       <c r="B317" s="20"/>
-      <c r="C317" s="13"/>
+      <c r="C317" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D317" s="39"/>
       <c r="E317" s="9"/>
       <c r="F317" s="20"/>
-      <c r="G317" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G317" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H317" s="39"/>
       <c r="I317" s="9"/>
@@ -9671,20 +9816,1248 @@
       <c r="K317" s="20"/>
     </row>
     <row r="318" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A318" s="41"/>
-      <c r="B318" s="15"/>
-      <c r="C318" s="42"/>
-      <c r="D318" s="43"/>
+      <c r="A318" s="40">
+        <v>44044</v>
+      </c>
+      <c r="B318" s="20"/>
+      <c r="C318" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D318" s="39"/>
       <c r="E318" s="9"/>
-      <c r="F318" s="15"/>
-      <c r="G318" s="42" t="str">
+      <c r="F318" s="20"/>
+      <c r="G318" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H318" s="39"/>
+      <c r="I318" s="9"/>
+      <c r="J318" s="11"/>
+      <c r="K318" s="20"/>
+    </row>
+    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A319" s="40">
+        <v>44075</v>
+      </c>
+      <c r="B319" s="20"/>
+      <c r="C319" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D319" s="39"/>
+      <c r="E319" s="9"/>
+      <c r="F319" s="20"/>
+      <c r="G319" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H319" s="39"/>
+      <c r="I319" s="9"/>
+      <c r="J319" s="11"/>
+      <c r="K319" s="20"/>
+    </row>
+    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A320" s="40">
+        <v>44105</v>
+      </c>
+      <c r="B320" s="15"/>
+      <c r="C320" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D320" s="43"/>
+      <c r="E320" s="9"/>
+      <c r="F320" s="15"/>
+      <c r="G320" s="42">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H320" s="43"/>
+      <c r="I320" s="9"/>
+      <c r="J320" s="12"/>
+      <c r="K320" s="15"/>
+    </row>
+    <row r="321" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A321" s="40">
+        <v>44136</v>
+      </c>
+      <c r="B321" s="20"/>
+      <c r="C321" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D321" s="39"/>
+      <c r="E321" s="9"/>
+      <c r="F321" s="20"/>
+      <c r="G321" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H321" s="39"/>
+      <c r="I321" s="9"/>
+      <c r="J321" s="11"/>
+      <c r="K321" s="20"/>
+    </row>
+    <row r="322" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A322" s="40">
+        <v>44166</v>
+      </c>
+      <c r="B322" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C322" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D322" s="39">
+        <v>5</v>
+      </c>
+      <c r="E322" s="9"/>
+      <c r="F322" s="20"/>
+      <c r="G322" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H322" s="39"/>
+      <c r="I322" s="9"/>
+      <c r="J322" s="11"/>
+      <c r="K322" s="20"/>
+    </row>
+    <row r="323" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A323" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="B323" s="20"/>
+      <c r="C323" s="13"/>
+      <c r="D323" s="39"/>
+      <c r="E323" s="9"/>
+      <c r="F323" s="20"/>
+      <c r="G323" s="13" t="str">
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H318" s="43"/>
-      <c r="I318" s="9"/>
-      <c r="J318" s="12"/>
-      <c r="K318" s="15"/>
+      <c r="H323" s="39"/>
+      <c r="I323" s="9"/>
+      <c r="J323" s="11"/>
+      <c r="K323" s="20"/>
+    </row>
+    <row r="324" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A324" s="40">
+        <v>44197</v>
+      </c>
+      <c r="B324" s="20"/>
+      <c r="C324" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D324" s="39"/>
+      <c r="E324" s="9"/>
+      <c r="F324" s="20"/>
+      <c r="G324" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H324" s="39"/>
+      <c r="I324" s="9"/>
+      <c r="J324" s="11"/>
+      <c r="K324" s="20"/>
+    </row>
+    <row r="325" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A325" s="40">
+        <v>44228</v>
+      </c>
+      <c r="B325" s="20"/>
+      <c r="C325" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D325" s="39"/>
+      <c r="E325" s="9"/>
+      <c r="F325" s="20"/>
+      <c r="G325" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H325" s="39"/>
+      <c r="I325" s="9"/>
+      <c r="J325" s="11"/>
+      <c r="K325" s="20"/>
+    </row>
+    <row r="326" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A326" s="40">
+        <v>44256</v>
+      </c>
+      <c r="B326" s="20"/>
+      <c r="C326" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D326" s="39"/>
+      <c r="E326" s="9"/>
+      <c r="F326" s="20"/>
+      <c r="G326" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H326" s="39"/>
+      <c r="I326" s="9"/>
+      <c r="J326" s="11"/>
+      <c r="K326" s="20"/>
+    </row>
+    <row r="327" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A327" s="40">
+        <v>44287</v>
+      </c>
+      <c r="B327" s="20"/>
+      <c r="C327" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D327" s="39"/>
+      <c r="E327" s="9"/>
+      <c r="F327" s="20"/>
+      <c r="G327" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H327" s="39"/>
+      <c r="I327" s="9"/>
+      <c r="J327" s="11"/>
+      <c r="K327" s="20"/>
+    </row>
+    <row r="328" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A328" s="40">
+        <v>44317</v>
+      </c>
+      <c r="B328" s="20"/>
+      <c r="C328" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D328" s="39"/>
+      <c r="E328" s="9"/>
+      <c r="F328" s="20"/>
+      <c r="G328" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H328" s="39"/>
+      <c r="I328" s="9"/>
+      <c r="J328" s="11"/>
+      <c r="K328" s="20"/>
+    </row>
+    <row r="329" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A329" s="40">
+        <v>44348</v>
+      </c>
+      <c r="B329" s="20"/>
+      <c r="C329" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D329" s="39"/>
+      <c r="E329" s="9"/>
+      <c r="F329" s="20"/>
+      <c r="G329" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H329" s="39"/>
+      <c r="I329" s="9"/>
+      <c r="J329" s="11"/>
+      <c r="K329" s="20"/>
+    </row>
+    <row r="330" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A330" s="40">
+        <v>44378</v>
+      </c>
+      <c r="B330" s="20"/>
+      <c r="C330" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D330" s="39"/>
+      <c r="E330" s="9"/>
+      <c r="F330" s="20"/>
+      <c r="G330" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H330" s="39"/>
+      <c r="I330" s="9"/>
+      <c r="J330" s="11"/>
+      <c r="K330" s="20"/>
+    </row>
+    <row r="331" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A331" s="40">
+        <v>44409</v>
+      </c>
+      <c r="B331" s="20"/>
+      <c r="C331" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D331" s="39"/>
+      <c r="E331" s="9"/>
+      <c r="F331" s="20"/>
+      <c r="G331" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H331" s="39"/>
+      <c r="I331" s="9"/>
+      <c r="J331" s="11"/>
+      <c r="K331" s="20"/>
+    </row>
+    <row r="332" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A332" s="40">
+        <v>44440</v>
+      </c>
+      <c r="B332" s="20"/>
+      <c r="C332" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D332" s="39"/>
+      <c r="E332" s="9"/>
+      <c r="F332" s="20"/>
+      <c r="G332" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H332" s="39"/>
+      <c r="I332" s="9"/>
+      <c r="J332" s="11"/>
+      <c r="K332" s="20"/>
+    </row>
+    <row r="333" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A333" s="40">
+        <v>44470</v>
+      </c>
+      <c r="B333" s="20"/>
+      <c r="C333" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D333" s="39"/>
+      <c r="E333" s="9"/>
+      <c r="F333" s="20"/>
+      <c r="G333" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H333" s="39"/>
+      <c r="I333" s="9"/>
+      <c r="J333" s="11"/>
+      <c r="K333" s="20"/>
+    </row>
+    <row r="334" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A334" s="40">
+        <v>44501</v>
+      </c>
+      <c r="B334" s="20"/>
+      <c r="C334" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D334" s="39"/>
+      <c r="E334" s="9"/>
+      <c r="F334" s="20"/>
+      <c r="G334" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H334" s="39"/>
+      <c r="I334" s="9"/>
+      <c r="J334" s="11"/>
+      <c r="K334" s="20"/>
+    </row>
+    <row r="335" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A335" s="40">
+        <v>44531</v>
+      </c>
+      <c r="B335" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C335" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D335" s="39">
+        <v>5</v>
+      </c>
+      <c r="E335" s="9"/>
+      <c r="F335" s="20"/>
+      <c r="G335" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H335" s="39"/>
+      <c r="I335" s="9"/>
+      <c r="J335" s="11"/>
+      <c r="K335" s="20"/>
+    </row>
+    <row r="336" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A336" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="B336" s="20"/>
+      <c r="C336" s="13"/>
+      <c r="D336" s="39"/>
+      <c r="E336" s="9"/>
+      <c r="F336" s="20"/>
+      <c r="G336" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H336" s="39"/>
+      <c r="I336" s="9"/>
+      <c r="J336" s="11"/>
+      <c r="K336" s="20"/>
+    </row>
+    <row r="337" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A337" s="40">
+        <v>44562</v>
+      </c>
+      <c r="B337" s="20"/>
+      <c r="C337" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D337" s="39"/>
+      <c r="E337" s="9"/>
+      <c r="F337" s="20"/>
+      <c r="G337" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H337" s="39"/>
+      <c r="I337" s="9"/>
+      <c r="J337" s="11"/>
+      <c r="K337" s="20"/>
+    </row>
+    <row r="338" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A338" s="40">
+        <v>44593</v>
+      </c>
+      <c r="B338" s="20"/>
+      <c r="C338" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D338" s="39"/>
+      <c r="E338" s="9"/>
+      <c r="F338" s="20"/>
+      <c r="G338" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H338" s="39"/>
+      <c r="I338" s="9"/>
+      <c r="J338" s="11"/>
+      <c r="K338" s="20"/>
+    </row>
+    <row r="339" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A339" s="40">
+        <v>44621</v>
+      </c>
+      <c r="B339" s="20"/>
+      <c r="C339" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D339" s="39"/>
+      <c r="E339" s="9"/>
+      <c r="F339" s="20"/>
+      <c r="G339" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H339" s="39"/>
+      <c r="I339" s="9"/>
+      <c r="J339" s="11"/>
+      <c r="K339" s="20"/>
+    </row>
+    <row r="340" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A340" s="40">
+        <v>44652</v>
+      </c>
+      <c r="B340" s="20"/>
+      <c r="C340" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D340" s="39"/>
+      <c r="E340" s="9"/>
+      <c r="F340" s="20"/>
+      <c r="G340" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H340" s="39"/>
+      <c r="I340" s="9"/>
+      <c r="J340" s="11"/>
+      <c r="K340" s="20"/>
+    </row>
+    <row r="341" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A341" s="40">
+        <v>44682</v>
+      </c>
+      <c r="B341" s="20"/>
+      <c r="C341" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D341" s="39"/>
+      <c r="E341" s="9"/>
+      <c r="F341" s="20"/>
+      <c r="G341" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H341" s="39"/>
+      <c r="I341" s="9"/>
+      <c r="J341" s="11"/>
+      <c r="K341" s="20"/>
+    </row>
+    <row r="342" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A342" s="40">
+        <v>44713</v>
+      </c>
+      <c r="B342" s="20"/>
+      <c r="C342" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D342" s="39"/>
+      <c r="E342" s="9"/>
+      <c r="F342" s="20"/>
+      <c r="G342" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H342" s="39"/>
+      <c r="I342" s="9"/>
+      <c r="J342" s="11"/>
+      <c r="K342" s="20"/>
+    </row>
+    <row r="343" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A343" s="40">
+        <v>44743</v>
+      </c>
+      <c r="B343" s="20"/>
+      <c r="C343" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D343" s="39"/>
+      <c r="E343" s="9"/>
+      <c r="F343" s="20"/>
+      <c r="G343" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H343" s="39"/>
+      <c r="I343" s="9"/>
+      <c r="J343" s="11"/>
+      <c r="K343" s="20"/>
+    </row>
+    <row r="344" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A344" s="40">
+        <v>44774</v>
+      </c>
+      <c r="B344" s="20"/>
+      <c r="C344" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D344" s="39"/>
+      <c r="E344" s="9"/>
+      <c r="F344" s="20"/>
+      <c r="G344" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H344" s="39"/>
+      <c r="I344" s="9"/>
+      <c r="J344" s="11"/>
+      <c r="K344" s="20"/>
+    </row>
+    <row r="345" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A345" s="40">
+        <v>44805</v>
+      </c>
+      <c r="B345" s="20"/>
+      <c r="C345" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D345" s="39"/>
+      <c r="E345" s="9"/>
+      <c r="F345" s="20"/>
+      <c r="G345" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H345" s="39"/>
+      <c r="I345" s="9"/>
+      <c r="J345" s="11"/>
+      <c r="K345" s="20"/>
+    </row>
+    <row r="346" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A346" s="40">
+        <v>44835</v>
+      </c>
+      <c r="B346" s="20"/>
+      <c r="C346" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D346" s="39"/>
+      <c r="E346" s="9"/>
+      <c r="F346" s="20"/>
+      <c r="G346" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H346" s="39"/>
+      <c r="I346" s="9"/>
+      <c r="J346" s="11"/>
+      <c r="K346" s="20"/>
+    </row>
+    <row r="347" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A347" s="40">
+        <v>44866</v>
+      </c>
+      <c r="B347" s="20"/>
+      <c r="C347" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D347" s="39"/>
+      <c r="E347" s="9"/>
+      <c r="F347" s="20"/>
+      <c r="G347" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H347" s="39"/>
+      <c r="I347" s="9"/>
+      <c r="J347" s="11"/>
+      <c r="K347" s="20"/>
+    </row>
+    <row r="348" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A348" s="40">
+        <v>44896</v>
+      </c>
+      <c r="B348" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C348" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D348" s="39">
+        <v>5</v>
+      </c>
+      <c r="E348" s="9"/>
+      <c r="F348" s="20"/>
+      <c r="G348" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H348" s="39"/>
+      <c r="I348" s="9"/>
+      <c r="J348" s="11"/>
+      <c r="K348" s="20"/>
+    </row>
+    <row r="349" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A349" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B349" s="20"/>
+      <c r="C349" s="13"/>
+      <c r="D349" s="39"/>
+      <c r="E349" s="9"/>
+      <c r="F349" s="20"/>
+      <c r="G349" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H349" s="39"/>
+      <c r="I349" s="9"/>
+      <c r="J349" s="11"/>
+      <c r="K349" s="20"/>
+    </row>
+    <row r="350" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A350" s="40">
+        <v>44927</v>
+      </c>
+      <c r="B350" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C350" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D350" s="39"/>
+      <c r="E350" s="9"/>
+      <c r="F350" s="20"/>
+      <c r="G350" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H350" s="39">
+        <v>10</v>
+      </c>
+      <c r="I350" s="9"/>
+      <c r="J350" s="11"/>
+      <c r="K350" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="351" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A351" s="40">
+        <v>44958</v>
+      </c>
+      <c r="B351" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="C351" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D351" s="39"/>
+      <c r="E351" s="9"/>
+      <c r="F351" s="20"/>
+      <c r="G351" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H351" s="39">
+        <v>20</v>
+      </c>
+      <c r="I351" s="9"/>
+      <c r="J351" s="11"/>
+      <c r="K351" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="352" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A352" s="40">
+        <v>44986</v>
+      </c>
+      <c r="B352" s="20"/>
+      <c r="C352" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D352" s="39"/>
+      <c r="E352" s="9"/>
+      <c r="F352" s="20"/>
+      <c r="G352" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H352" s="39"/>
+      <c r="I352" s="9"/>
+      <c r="J352" s="11"/>
+      <c r="K352" s="20"/>
+    </row>
+    <row r="353" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A353" s="40">
+        <v>45017</v>
+      </c>
+      <c r="B353" s="20"/>
+      <c r="C353" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D353" s="39"/>
+      <c r="E353" s="9"/>
+      <c r="F353" s="20"/>
+      <c r="G353" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H353" s="39"/>
+      <c r="I353" s="9"/>
+      <c r="J353" s="11"/>
+      <c r="K353" s="20"/>
+    </row>
+    <row r="354" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A354" s="40">
+        <v>45047</v>
+      </c>
+      <c r="B354" s="20"/>
+      <c r="C354" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="D354" s="39"/>
+      <c r="E354" s="9"/>
+      <c r="F354" s="20"/>
+      <c r="G354" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
+      </c>
+      <c r="H354" s="39"/>
+      <c r="I354" s="9"/>
+      <c r="J354" s="11"/>
+      <c r="K354" s="20"/>
+    </row>
+    <row r="355" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A355" s="40">
+        <v>45078</v>
+      </c>
+      <c r="B355" s="20"/>
+      <c r="C355" s="13"/>
+      <c r="D355" s="39"/>
+      <c r="E355" s="9"/>
+      <c r="F355" s="20"/>
+      <c r="G355" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H355" s="39"/>
+      <c r="I355" s="9"/>
+      <c r="J355" s="11"/>
+      <c r="K355" s="20"/>
+    </row>
+    <row r="356" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A356" s="40">
+        <v>45108</v>
+      </c>
+      <c r="B356" s="20"/>
+      <c r="C356" s="13"/>
+      <c r="D356" s="39"/>
+      <c r="E356" s="9"/>
+      <c r="F356" s="20"/>
+      <c r="G356" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H356" s="39"/>
+      <c r="I356" s="9"/>
+      <c r="J356" s="11"/>
+      <c r="K356" s="20"/>
+    </row>
+    <row r="357" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A357" s="40">
+        <v>45139</v>
+      </c>
+      <c r="B357" s="20"/>
+      <c r="C357" s="13"/>
+      <c r="D357" s="39"/>
+      <c r="E357" s="9"/>
+      <c r="F357" s="20"/>
+      <c r="G357" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H357" s="39"/>
+      <c r="I357" s="9"/>
+      <c r="J357" s="11"/>
+      <c r="K357" s="20"/>
+    </row>
+    <row r="358" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A358" s="40">
+        <v>45170</v>
+      </c>
+      <c r="B358" s="20"/>
+      <c r="C358" s="13"/>
+      <c r="D358" s="39"/>
+      <c r="E358" s="9"/>
+      <c r="F358" s="20"/>
+      <c r="G358" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H358" s="39"/>
+      <c r="I358" s="9"/>
+      <c r="J358" s="11"/>
+      <c r="K358" s="20"/>
+    </row>
+    <row r="359" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A359" s="40">
+        <v>45200</v>
+      </c>
+      <c r="B359" s="20"/>
+      <c r="C359" s="13"/>
+      <c r="D359" s="39"/>
+      <c r="E359" s="9"/>
+      <c r="F359" s="20"/>
+      <c r="G359" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H359" s="39"/>
+      <c r="I359" s="9"/>
+      <c r="J359" s="11"/>
+      <c r="K359" s="20"/>
+    </row>
+    <row r="360" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A360" s="40">
+        <v>45231</v>
+      </c>
+      <c r="B360" s="20"/>
+      <c r="C360" s="13"/>
+      <c r="D360" s="39"/>
+      <c r="E360" s="9"/>
+      <c r="F360" s="20"/>
+      <c r="G360" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H360" s="39"/>
+      <c r="I360" s="9"/>
+      <c r="J360" s="11"/>
+      <c r="K360" s="20"/>
+    </row>
+    <row r="361" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A361" s="40">
+        <v>45261</v>
+      </c>
+      <c r="B361" s="20"/>
+      <c r="C361" s="13"/>
+      <c r="D361" s="39"/>
+      <c r="E361" s="9"/>
+      <c r="F361" s="20"/>
+      <c r="G361" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H361" s="39"/>
+      <c r="I361" s="9"/>
+      <c r="J361" s="11"/>
+      <c r="K361" s="20"/>
+    </row>
+    <row r="362" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A362" s="40">
+        <v>45292</v>
+      </c>
+      <c r="B362" s="20"/>
+      <c r="C362" s="13"/>
+      <c r="D362" s="39"/>
+      <c r="E362" s="9"/>
+      <c r="F362" s="20"/>
+      <c r="G362" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H362" s="39"/>
+      <c r="I362" s="9"/>
+      <c r="J362" s="11"/>
+      <c r="K362" s="20"/>
+    </row>
+    <row r="363" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A363" s="40">
+        <v>45323</v>
+      </c>
+      <c r="B363" s="20"/>
+      <c r="C363" s="13"/>
+      <c r="D363" s="39"/>
+      <c r="E363" s="9"/>
+      <c r="F363" s="20"/>
+      <c r="G363" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H363" s="39"/>
+      <c r="I363" s="9"/>
+      <c r="J363" s="11"/>
+      <c r="K363" s="20"/>
+    </row>
+    <row r="364" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A364" s="40">
+        <v>45352</v>
+      </c>
+      <c r="B364" s="20"/>
+      <c r="C364" s="13"/>
+      <c r="D364" s="39"/>
+      <c r="E364" s="9"/>
+      <c r="F364" s="20"/>
+      <c r="G364" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H364" s="39"/>
+      <c r="I364" s="9"/>
+      <c r="J364" s="11"/>
+      <c r="K364" s="20"/>
+    </row>
+    <row r="365" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A365" s="40">
+        <v>45383</v>
+      </c>
+      <c r="B365" s="20"/>
+      <c r="C365" s="13"/>
+      <c r="D365" s="39"/>
+      <c r="E365" s="9"/>
+      <c r="F365" s="20"/>
+      <c r="G365" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H365" s="39"/>
+      <c r="I365" s="9"/>
+      <c r="J365" s="11"/>
+      <c r="K365" s="20"/>
+    </row>
+    <row r="366" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A366" s="40">
+        <v>45413</v>
+      </c>
+      <c r="B366" s="20"/>
+      <c r="C366" s="13"/>
+      <c r="D366" s="39"/>
+      <c r="E366" s="9"/>
+      <c r="F366" s="20"/>
+      <c r="G366" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H366" s="39"/>
+      <c r="I366" s="9"/>
+      <c r="J366" s="11"/>
+      <c r="K366" s="20"/>
+    </row>
+    <row r="367" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A367" s="40">
+        <v>45444</v>
+      </c>
+      <c r="B367" s="20"/>
+      <c r="C367" s="13"/>
+      <c r="D367" s="39"/>
+      <c r="E367" s="9"/>
+      <c r="F367" s="20"/>
+      <c r="G367" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H367" s="39"/>
+      <c r="I367" s="9"/>
+      <c r="J367" s="11"/>
+      <c r="K367" s="20"/>
+    </row>
+    <row r="368" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A368" s="40">
+        <v>45474</v>
+      </c>
+      <c r="B368" s="20"/>
+      <c r="C368" s="13"/>
+      <c r="D368" s="39"/>
+      <c r="E368" s="9"/>
+      <c r="F368" s="20"/>
+      <c r="G368" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H368" s="39"/>
+      <c r="I368" s="9"/>
+      <c r="J368" s="11"/>
+      <c r="K368" s="20"/>
+    </row>
+    <row r="369" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A369" s="40">
+        <v>45505</v>
+      </c>
+      <c r="B369" s="20"/>
+      <c r="C369" s="13"/>
+      <c r="D369" s="39"/>
+      <c r="E369" s="9"/>
+      <c r="F369" s="20"/>
+      <c r="G369" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H369" s="39"/>
+      <c r="I369" s="9"/>
+      <c r="J369" s="11"/>
+      <c r="K369" s="20"/>
+    </row>
+    <row r="370" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A370" s="40">
+        <v>45536</v>
+      </c>
+      <c r="B370" s="20"/>
+      <c r="C370" s="13"/>
+      <c r="D370" s="39"/>
+      <c r="E370" s="9"/>
+      <c r="F370" s="20"/>
+      <c r="G370" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H370" s="39"/>
+      <c r="I370" s="9"/>
+      <c r="J370" s="11"/>
+      <c r="K370" s="20"/>
+    </row>
+    <row r="371" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A371" s="40">
+        <v>45566</v>
+      </c>
+      <c r="B371" s="20"/>
+      <c r="C371" s="13"/>
+      <c r="D371" s="39"/>
+      <c r="E371" s="9"/>
+      <c r="F371" s="20"/>
+      <c r="G371" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H371" s="39"/>
+      <c r="I371" s="9"/>
+      <c r="J371" s="11"/>
+      <c r="K371" s="20"/>
+    </row>
+    <row r="372" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A372" s="40">
+        <v>45597</v>
+      </c>
+      <c r="B372" s="20"/>
+      <c r="C372" s="13"/>
+      <c r="D372" s="39"/>
+      <c r="E372" s="9"/>
+      <c r="F372" s="20"/>
+      <c r="G372" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H372" s="39"/>
+      <c r="I372" s="9"/>
+      <c r="J372" s="11"/>
+      <c r="K372" s="20"/>
+    </row>
+    <row r="373" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A373" s="40">
+        <v>45627</v>
+      </c>
+      <c r="B373" s="20"/>
+      <c r="C373" s="13"/>
+      <c r="D373" s="39"/>
+      <c r="E373" s="9"/>
+      <c r="F373" s="20"/>
+      <c r="G373" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H373" s="39"/>
+      <c r="I373" s="9"/>
+      <c r="J373" s="11"/>
+      <c r="K373" s="20"/>
+    </row>
+    <row r="374" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A374" s="40">
+        <v>45658</v>
+      </c>
+      <c r="B374" s="20"/>
+      <c r="C374" s="13"/>
+      <c r="D374" s="39"/>
+      <c r="E374" s="9"/>
+      <c r="F374" s="20"/>
+      <c r="G374" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H374" s="39"/>
+      <c r="I374" s="9"/>
+      <c r="J374" s="11"/>
+      <c r="K374" s="20"/>
+    </row>
+    <row r="375" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A375" s="40">
+        <v>45689</v>
+      </c>
+      <c r="B375" s="20"/>
+      <c r="C375" s="13"/>
+      <c r="D375" s="39"/>
+      <c r="E375" s="9"/>
+      <c r="F375" s="20"/>
+      <c r="G375" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H375" s="39"/>
+      <c r="I375" s="9"/>
+      <c r="J375" s="11"/>
+      <c r="K375" s="20"/>
+    </row>
+    <row r="376" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A376" s="40">
+        <v>45717</v>
+      </c>
+      <c r="B376" s="20"/>
+      <c r="C376" s="13"/>
+      <c r="D376" s="39"/>
+      <c r="E376" s="9"/>
+      <c r="F376" s="20"/>
+      <c r="G376" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H376" s="39"/>
+      <c r="I376" s="9"/>
+      <c r="J376" s="11"/>
+      <c r="K376" s="20"/>
+    </row>
+    <row r="377" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A377" s="40">
+        <v>45748</v>
+      </c>
+      <c r="B377" s="20"/>
+      <c r="C377" s="13"/>
+      <c r="D377" s="39"/>
+      <c r="E377" s="9"/>
+      <c r="F377" s="20"/>
+      <c r="G377" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H377" s="39"/>
+      <c r="I377" s="9"/>
+      <c r="J377" s="11"/>
+      <c r="K377" s="20"/>
+    </row>
+    <row r="378" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A378" s="40">
+        <v>45778</v>
+      </c>
+      <c r="B378" s="20"/>
+      <c r="C378" s="13"/>
+      <c r="D378" s="39"/>
+      <c r="E378" s="9"/>
+      <c r="F378" s="20"/>
+      <c r="G378" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H378" s="39"/>
+      <c r="I378" s="9"/>
+      <c r="J378" s="11"/>
+      <c r="K378" s="20"/>
+    </row>
+    <row r="379" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A379" s="40">
+        <v>45809</v>
+      </c>
+      <c r="B379" s="20"/>
+      <c r="C379" s="13"/>
+      <c r="D379" s="39"/>
+      <c r="E379" s="9"/>
+      <c r="F379" s="20"/>
+      <c r="G379" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H379" s="39"/>
+      <c r="I379" s="9"/>
+      <c r="J379" s="11"/>
+      <c r="K379" s="20"/>
+    </row>
+    <row r="380" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A380" s="40">
+        <v>45839</v>
+      </c>
+      <c r="B380" s="20"/>
+      <c r="C380" s="13"/>
+      <c r="D380" s="39"/>
+      <c r="E380" s="9"/>
+      <c r="F380" s="20"/>
+      <c r="G380" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H380" s="39"/>
+      <c r="I380" s="9"/>
+      <c r="J380" s="11"/>
+      <c r="K380" s="20"/>
+    </row>
+    <row r="381" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A381" s="40">
+        <v>45870</v>
+      </c>
+      <c r="B381" s="20"/>
+      <c r="C381" s="13"/>
+      <c r="D381" s="39"/>
+      <c r="E381" s="9"/>
+      <c r="F381" s="20"/>
+      <c r="G381" s="13" t="str">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H381" s="39"/>
+      <c r="I381" s="9"/>
+      <c r="J381" s="11"/>
+      <c r="K381" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -9700,11 +11073,11 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F4:G4"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9727,7 +11100,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L67"/>
   <sheetViews>
@@ -9750,17 +11123,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="J1" s="59" t="s">
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="J1" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
@@ -9841,12 +11214,12 @@
         <v>30</v>
       </c>
       <c r="G6" s="44"/>
-      <c r="I6" s="59" t="s">
+      <c r="I6" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" s="37">

</xml_diff>